<commit_message>
revisi menrevisi kombinasi loc
</commit_message>
<xml_diff>
--- a/xlsx/nfeature: 1024, hamming_tolerance: 32, k_knn: 15.xlsx
+++ b/xlsx/nfeature: 1024, hamming_tolerance: 32, k_knn: 15.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,7 +428,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.548</v>
+        <v>0.351</v>
       </c>
       <c r="C1" t="n">
         <v>0.001</v>
@@ -457,13 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9330000000000001</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="C2" t="n">
         <v>0.002</v>
       </c>
       <c r="D2" t="n">
-        <v>0.397</v>
+        <v>0.398</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9320000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="C3" t="n">
         <v>0.002</v>
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.531</v>
+        <v>0.334</v>
       </c>
       <c r="C4" t="n">
         <v>0.001</v>
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.535</v>
+        <v>0.32</v>
       </c>
       <c r="C5" t="n">
         <v>0.001</v>
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.911</v>
+        <v>1.343</v>
       </c>
       <c r="C6" t="n">
         <v>0.004</v>
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.397</v>
+        <v>1.03</v>
       </c>
       <c r="C7" t="n">
         <v>0.003</v>
       </c>
       <c r="D7" t="n">
-        <v>0.316</v>
+        <v>0.311</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8</v>
+        <v>0.867</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -631,13 +631,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.965</v>
+        <v>1.568</v>
       </c>
       <c r="C8" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="D8" t="n">
-        <v>0.632</v>
+        <v>0.627</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -660,16 +660,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.423</v>
+        <v>0.987</v>
       </c>
       <c r="C9" t="n">
         <v>0.003</v>
       </c>
       <c r="D9" t="n">
-        <v>0.216</v>
+        <v>0.223</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -689,13 +689,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.913</v>
+        <v>1.378</v>
       </c>
       <c r="C10" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="D10" t="n">
-        <v>0.267</v>
+        <v>0.247</v>
       </c>
       <c r="E10" t="n">
         <v>0.9330000000000001</v>
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.855</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="C11" t="n">
         <v>0.002</v>
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.263</v>
+        <v>0.949</v>
       </c>
       <c r="C12" t="n">
         <v>0.003</v>
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.898</v>
+        <v>0.718</v>
       </c>
       <c r="C13" t="n">
         <v>0.002</v>
@@ -805,10 +805,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.059</v>
+        <v>0.759</v>
       </c>
       <c r="C14" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="D14" t="n">
         <v>0.488</v>
@@ -834,25 +834,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.069</v>
+        <v>0.791</v>
       </c>
       <c r="C15" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="D15" t="n">
-        <v>0.505</v>
+        <v>0.413</v>
       </c>
       <c r="E15" t="n">
-        <v>0.467</v>
+        <v>0.667</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Tidak Diketahui</t>
+          <t>Toni Ismail</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Salah</t>
+          <t>Benar</t>
         </is>
       </c>
     </row>
@@ -863,13 +863,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.268</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="C16" t="n">
         <v>0.002</v>
       </c>
       <c r="D16" t="n">
-        <v>0.677</v>
+        <v>0.676</v>
       </c>
       <c r="E16" t="n">
         <v>0.667</v>
@@ -892,13 +892,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.821</v>
+        <v>0.532</v>
       </c>
       <c r="C17" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="D17" t="n">
-        <v>0.382</v>
+        <v>0.383</v>
       </c>
       <c r="E17" t="n">
         <v>0.8</v>
@@ -921,13 +921,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.209</v>
+        <v>0.88</v>
       </c>
       <c r="C18" t="n">
         <v>0.003</v>
       </c>
       <c r="D18" t="n">
-        <v>0.45</v>
+        <v>0.449</v>
       </c>
       <c r="E18" t="n">
         <v>0.667</v>
@@ -950,13 +950,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.702</v>
+        <v>0.469</v>
       </c>
       <c r="C19" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="D19" t="n">
-        <v>0.446</v>
+        <v>0.445</v>
       </c>
       <c r="E19" t="n">
         <v>0.533</v>
@@ -979,16 +979,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.134</v>
+        <v>0.864</v>
       </c>
       <c r="C20" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="D20" t="n">
-        <v>0.315</v>
+        <v>0.294</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8</v>
+        <v>0.867</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1008,13 +1008,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.611</v>
+        <v>0.372</v>
       </c>
       <c r="C21" t="n">
         <v>0.001</v>
       </c>
       <c r="D21" t="n">
-        <v>0.344</v>
+        <v>0.343</v>
       </c>
       <c r="E21" t="n">
         <v>0.467</v>
@@ -1037,13 +1037,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.655</v>
+        <v>1.075</v>
       </c>
       <c r="C22" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="D22" t="n">
-        <v>0.174</v>
+        <v>0.169</v>
       </c>
       <c r="E22" t="n">
         <v>0.4</v>
@@ -1066,16 +1066,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.272</v>
+        <v>1.009</v>
       </c>
       <c r="C23" t="n">
         <v>0.003</v>
       </c>
       <c r="D23" t="n">
-        <v>0.388</v>
+        <v>0.362</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9330000000000001</v>
+        <v>1</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1095,13 +1095,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1.569</v>
+        <v>1.302</v>
       </c>
       <c r="C24" t="n">
         <v>0.004</v>
       </c>
       <c r="D24" t="n">
-        <v>0.506</v>
+        <v>0.482</v>
       </c>
       <c r="E24" t="n">
         <v>0.9330000000000001</v>
@@ -1124,13 +1124,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.485</v>
+        <v>1.265</v>
       </c>
       <c r="C25" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="D25" t="n">
-        <v>0.55</v>
+        <v>0.52</v>
       </c>
       <c r="E25" t="n">
         <v>0.9330000000000001</v>
@@ -1153,16 +1153,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.278</v>
+        <v>0.926</v>
       </c>
       <c r="C26" t="n">
         <v>0.003</v>
       </c>
       <c r="D26" t="n">
-        <v>0.108</v>
+        <v>0.106</v>
       </c>
       <c r="E26" t="n">
-        <v>0.8</v>
+        <v>0.867</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1182,13 +1182,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.523</v>
+        <v>1.228</v>
       </c>
       <c r="C27" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="D27" t="n">
-        <v>0.544</v>
+        <v>0.526</v>
       </c>
       <c r="E27" t="n">
         <v>0.867</v>
@@ -1211,13 +1211,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1.638</v>
+        <v>1.282</v>
       </c>
       <c r="C28" t="n">
         <v>0.004</v>
       </c>
       <c r="D28" t="n">
-        <v>0.569</v>
+        <v>0.544</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
@@ -1240,7 +1240,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.867</v>
+        <v>0.679</v>
       </c>
       <c r="C29" t="n">
         <v>0.002</v>
@@ -1269,13 +1269,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1.651</v>
+        <v>1.439</v>
       </c>
       <c r="C30" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="D30" t="n">
-        <v>0.553</v>
+        <v>0.55</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -1298,16 +1298,16 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.496</v>
       </c>
       <c r="C31" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="D31" t="n">
-        <v>0.286</v>
+        <v>0.275</v>
       </c>
       <c r="E31" t="n">
-        <v>0.8</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1327,13 +1327,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.839</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="C32" t="n">
         <v>0.002</v>
       </c>
       <c r="D32" t="n">
-        <v>0.189</v>
+        <v>0.188</v>
       </c>
       <c r="E32" t="n">
         <v>0.733</v>
@@ -1356,25 +1356,25 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1.02</v>
+        <v>0.986</v>
       </c>
       <c r="C33" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="D33" t="n">
-        <v>0.168</v>
+        <v>0.308</v>
       </c>
       <c r="E33" t="n">
-        <v>0.467</v>
+        <v>0.733</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Tidak Diketahui</t>
+          <t>Fanny Yusuf</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Salah</t>
+          <t>Benar</t>
         </is>
       </c>
     </row>
@@ -1385,16 +1385,16 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.965</v>
+        <v>1.478</v>
       </c>
       <c r="C34" t="n">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="D34" t="n">
-        <v>0.191</v>
+        <v>0.481</v>
       </c>
       <c r="E34" t="n">
-        <v>0.867</v>
+        <v>0.6</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1414,16 +1414,16 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1.634</v>
+        <v>1.381</v>
       </c>
       <c r="C35" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="D35" t="n">
-        <v>0.546</v>
+        <v>0.468</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1439,24 +1439,24 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>TO_1.png</t>
+          <t>FY_4.png</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1.188</v>
+        <v>1.196</v>
       </c>
       <c r="C36" t="n">
-        <v>0.002</v>
+        <v>0.004</v>
       </c>
       <c r="D36" t="n">
-        <v>0.408</v>
+        <v>0.376</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Tiara Oktavian</t>
+          <t>Fanny Yusuf</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1468,20 +1468,20 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TO_2.png</t>
+          <t>TO_1.png</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1.243</v>
+        <v>0.624</v>
       </c>
       <c r="C37" t="n">
         <v>0.002</v>
       </c>
       <c r="D37" t="n">
-        <v>0.396</v>
+        <v>0.397</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1497,17 +1497,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>TO_3.png</t>
+          <t>TO_2.png</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1.1</v>
+        <v>0.898</v>
       </c>
       <c r="C38" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="D38" t="n">
-        <v>0.403</v>
+        <v>0.374</v>
       </c>
       <c r="E38" t="n">
         <v>1</v>
@@ -1526,49 +1526,49 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TO_4.png</t>
+          <t>TO_3.png</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2.292</v>
+        <v>0.657</v>
       </c>
       <c r="C39" t="n">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="D39" t="n">
-        <v>0.12</v>
+        <v>0.391</v>
       </c>
       <c r="E39" t="n">
-        <v>0.667</v>
+        <v>1</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Fanny Yusuf</t>
+          <t>Tiara Oktavian</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Salah</t>
+          <t>Benar</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>TO_5.png</t>
+          <t>TO_4.png</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1.167</v>
+        <v>2.874</v>
       </c>
       <c r="C40" t="n">
-        <v>0.002</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="D40" t="n">
-        <v>0.372</v>
+        <v>0.121</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1584,24 +1584,24 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TD_1.png</t>
+          <t>TO_5.png</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>4.262</v>
+        <v>2.803</v>
       </c>
       <c r="C41" t="n">
-        <v>0.006</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="D41" t="n">
-        <v>0.028</v>
+        <v>0.091</v>
       </c>
       <c r="E41" t="n">
-        <v>0.333</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Tidak Diketahui</t>
+          <t>Tiara Oktavian</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1613,20 +1613,20 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TD_2.png</t>
+          <t>TD_1.png</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4.463</v>
+        <v>2.132</v>
       </c>
       <c r="C42" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="D42" t="n">
-        <v>0.066</v>
+        <v>0.033</v>
       </c>
       <c r="E42" t="n">
-        <v>0.267</v>
+        <v>0.333</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1642,20 +1642,20 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TD_3.png</t>
+          <t>TD_2.png</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>1.333</v>
+        <v>2.297</v>
       </c>
       <c r="C43" t="n">
-        <v>0.002</v>
+        <v>0.008</v>
       </c>
       <c r="D43" t="n">
-        <v>0.199</v>
+        <v>0.059</v>
       </c>
       <c r="E43" t="n">
-        <v>0.4</v>
+        <v>0.267</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1671,29 +1671,58 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>TD_3.png</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.193</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Benar</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>TD_4.png</t>
         </is>
       </c>
-      <c r="B44" t="n">
-        <v>1.063</v>
-      </c>
-      <c r="C44" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0.123</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Fanny Yusuf</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Salah</t>
+      <c r="B45" t="n">
+        <v>0.796</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Benar</t>
         </is>
       </c>
     </row>

</xml_diff>